<commit_message>
all data from 2020 season
</commit_message>
<xml_diff>
--- a/Geelong_stats.xlsx
+++ b/Geelong_stats.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:IA102"/>
+  <dimension ref="A1:IC102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,6 +1061,12 @@
       <c r="IA1" t="n">
         <v>10323</v>
       </c>
+      <c r="IB1" t="n">
+        <v>10325</v>
+      </c>
+      <c r="IC1" t="n">
+        <v>10326</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1770,6 +1776,12 @@
       <c r="IA2" t="n">
         <v>2020</v>
       </c>
+      <c r="IB2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="IC2" t="n">
+        <v>2020</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2479,6 +2491,12 @@
       <c r="IA3" t="n">
         <v>26</v>
       </c>
+      <c r="IB3" t="n">
+        <v>27</v>
+      </c>
+      <c r="IC3" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3188,6 +3206,12 @@
       <c r="IA4" t="n">
         <v>0</v>
       </c>
+      <c r="IB4" t="n">
+        <v>1</v>
+      </c>
+      <c r="IC4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3897,6 +3921,12 @@
       <c r="IA5" t="n">
         <v>0</v>
       </c>
+      <c r="IB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="IC5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4606,6 +4636,12 @@
       <c r="IA6" t="n">
         <v>100</v>
       </c>
+      <c r="IB6" t="n">
+        <v>82</v>
+      </c>
+      <c r="IC6" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5315,6 +5351,12 @@
       <c r="IA7" t="n">
         <v>32</v>
       </c>
+      <c r="IB7" t="n">
+        <v>42</v>
+      </c>
+      <c r="IC7" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -6024,6 +6066,12 @@
       <c r="IA8" t="n">
         <v>68</v>
       </c>
+      <c r="IB8" t="n">
+        <v>40</v>
+      </c>
+      <c r="IC8" t="n">
+        <v>-31</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -6733,6 +6781,12 @@
       <c r="IA9" t="n">
         <v>1</v>
       </c>
+      <c r="IB9" t="n">
+        <v>1</v>
+      </c>
+      <c r="IC9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7442,6 +7496,12 @@
       <c r="IA10" t="n">
         <v>4</v>
       </c>
+      <c r="IB10" t="n">
+        <v>2</v>
+      </c>
+      <c r="IC10" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8151,6 +8211,12 @@
       <c r="IA11" t="n">
         <v>228</v>
       </c>
+      <c r="IB11" t="n">
+        <v>186</v>
+      </c>
+      <c r="IC11" t="n">
+        <v>161</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8860,6 +8926,12 @@
       <c r="IA12" t="n">
         <v>130</v>
       </c>
+      <c r="IB12" t="n">
+        <v>114</v>
+      </c>
+      <c r="IC12" t="n">
+        <v>113</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -9569,6 +9641,12 @@
       <c r="IA13" t="n">
         <v>358</v>
       </c>
+      <c r="IB13" t="n">
+        <v>300</v>
+      </c>
+      <c r="IC13" t="n">
+        <v>274</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -10278,6 +10356,12 @@
       <c r="IA14" t="n">
         <v>1.75</v>
       </c>
+      <c r="IB14" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="IC14" t="n">
+        <v>1.42</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -10987,6 +11071,12 @@
       <c r="IA15" t="n">
         <v>134</v>
       </c>
+      <c r="IB15" t="n">
+        <v>76</v>
+      </c>
+      <c r="IC15" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -11696,6 +11786,12 @@
       <c r="IA16" t="n">
         <v>46</v>
       </c>
+      <c r="IB16" t="n">
+        <v>56</v>
+      </c>
+      <c r="IC16" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -12405,6 +12501,12 @@
       <c r="IA17" t="n">
         <v>19</v>
       </c>
+      <c r="IB17" t="n">
+        <v>38</v>
+      </c>
+      <c r="IC17" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -13114,6 +13216,12 @@
       <c r="IA18" t="n">
         <v>13</v>
       </c>
+      <c r="IB18" t="n">
+        <v>7</v>
+      </c>
+      <c r="IC18" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -13823,6 +13931,12 @@
       <c r="IA19" t="n">
         <v>10</v>
       </c>
+      <c r="IB19" t="n">
+        <v>13</v>
+      </c>
+      <c r="IC19" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -14532,6 +14646,12 @@
       <c r="IA20" t="n">
         <v>15</v>
       </c>
+      <c r="IB20" t="n">
+        <v>11</v>
+      </c>
+      <c r="IC20" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -15241,6 +15361,12 @@
       <c r="IA21" t="n">
         <v>12</v>
       </c>
+      <c r="IB21" t="n">
+        <v>9</v>
+      </c>
+      <c r="IC21" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -15950,6 +16076,12 @@
       <c r="IA22" t="n">
         <v>7</v>
       </c>
+      <c r="IB22" t="n">
+        <v>11</v>
+      </c>
+      <c r="IC22" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -16659,6 +16791,12 @@
       <c r="IA23" t="n">
         <v>3</v>
       </c>
+      <c r="IB23" t="n">
+        <v>5</v>
+      </c>
+      <c r="IC23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -17368,6 +17506,12 @@
       <c r="IA24" t="n">
         <v>25</v>
       </c>
+      <c r="IB24" t="n">
+        <v>27</v>
+      </c>
+      <c r="IC24" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -18077,6 +18221,12 @@
       <c r="IA25" t="n">
         <v>60</v>
       </c>
+      <c r="IB25" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="IC25" t="n">
+        <v>46.7</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -18786,6 +18936,12 @@
       <c r="IA26" t="n">
         <v>23.87</v>
       </c>
+      <c r="IB26" t="n">
+        <v>27.27</v>
+      </c>
+      <c r="IC26" t="n">
+        <v>39.14</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -19495,6 +19651,12 @@
       <c r="IA27" t="n">
         <v>14.32</v>
       </c>
+      <c r="IB27" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="IC27" t="n">
+        <v>18.27</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -20204,6 +20366,12 @@
       <c r="IA28" t="n">
         <v>34</v>
       </c>
+      <c r="IB28" t="n">
+        <v>36</v>
+      </c>
+      <c r="IC28" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -20913,6 +21081,12 @@
       <c r="IA29" t="n">
         <v>37</v>
       </c>
+      <c r="IB29" t="n">
+        <v>42</v>
+      </c>
+      <c r="IC29" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -21622,6 +21796,12 @@
       <c r="IA30" t="n">
         <v>25</v>
       </c>
+      <c r="IB30" t="n">
+        <v>24</v>
+      </c>
+      <c r="IC30" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -22331,6 +22511,12 @@
       <c r="IA31" t="n">
         <v>46</v>
       </c>
+      <c r="IB31" t="n">
+        <v>50</v>
+      </c>
+      <c r="IC31" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -23040,6 +23226,12 @@
       <c r="IA32" t="n">
         <v>1.84</v>
       </c>
+      <c r="IB32" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="IC32" t="n">
+        <v>2.67</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -23749,6 +23941,12 @@
       <c r="IA33" t="n">
         <v>3.07</v>
       </c>
+      <c r="IB33" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="IC33" t="n">
+        <v>5.71</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -24458,6 +24656,12 @@
       <c r="IA34" t="n">
         <v>47.8</v>
       </c>
+      <c r="IB34" t="n">
+        <v>44</v>
+      </c>
+      <c r="IC34" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -25167,6 +25371,12 @@
       <c r="IA35" t="n">
         <v>32.6</v>
       </c>
+      <c r="IB35" t="n">
+        <v>22</v>
+      </c>
+      <c r="IC35" t="n">
+        <v>17.5</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -25876,6 +26086,12 @@
       <c r="IA36" t="n">
         <v>188.6</v>
       </c>
+      <c r="IB36" t="n">
+        <v>188.6</v>
+      </c>
+      <c r="IC36" t="n">
+        <v>188.6</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -26585,6 +26801,12 @@
       <c r="IA37" t="n">
         <v>89.3</v>
       </c>
+      <c r="IB37" t="n">
+        <v>89.3</v>
+      </c>
+      <c r="IC37" t="n">
+        <v>89.3</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -27294,6 +27516,12 @@
       <c r="IA38" t="n">
         <v>28.24</v>
       </c>
+      <c r="IB38" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="IC38" t="n">
+        <v>28.33</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -28003,6 +28231,12 @@
       <c r="IA39" t="n">
         <v>160.9</v>
       </c>
+      <c r="IB39" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="IC39" t="n">
+        <v>162.9</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -28712,6 +28946,12 @@
       <c r="IA40" t="n">
         <v>3</v>
       </c>
+      <c r="IB40" t="n">
+        <v>2</v>
+      </c>
+      <c r="IC40" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -29421,6 +29661,12 @@
       <c r="IA41" t="n">
         <v>4</v>
       </c>
+      <c r="IB41" t="n">
+        <v>5</v>
+      </c>
+      <c r="IC41" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -30130,6 +30376,12 @@
       <c r="IA42" t="n">
         <v>4</v>
       </c>
+      <c r="IB42" t="n">
+        <v>4</v>
+      </c>
+      <c r="IC42" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -30839,6 +31091,12 @@
       <c r="IA43" t="n">
         <v>11</v>
       </c>
+      <c r="IB43" t="n">
+        <v>11</v>
+      </c>
+      <c r="IC43" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -31548,6 +31806,12 @@
       <c r="IA44" t="n">
         <v>107</v>
       </c>
+      <c r="IB44" t="n">
+        <v>118</v>
+      </c>
+      <c r="IC44" t="n">
+        <v>124</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -32257,6 +32521,12 @@
       <c r="IA45" t="n">
         <v>251</v>
       </c>
+      <c r="IB45" t="n">
+        <v>177</v>
+      </c>
+      <c r="IC45" t="n">
+        <v>145</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -32966,6 +33236,12 @@
       <c r="IA46" t="n">
         <v>287</v>
       </c>
+      <c r="IB46" t="n">
+        <v>214</v>
+      </c>
+      <c r="IC46" t="n">
+        <v>169</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -33675,6 +33951,12 @@
       <c r="IA47" t="n">
         <v>80.2</v>
       </c>
+      <c r="IB47" t="n">
+        <v>71.3</v>
+      </c>
+      <c r="IC47" t="n">
+        <v>61.7</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -34384,6 +34666,12 @@
       <c r="IA48" t="n">
         <v>37</v>
       </c>
+      <c r="IB48" t="n">
+        <v>42</v>
+      </c>
+      <c r="IC48" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -35093,6 +35381,12 @@
       <c r="IA49" t="n">
         <v>14</v>
       </c>
+      <c r="IB49" t="n">
+        <v>7</v>
+      </c>
+      <c r="IC49" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -35802,6 +36096,12 @@
       <c r="IA50" t="n">
         <v>17</v>
       </c>
+      <c r="IB50" t="n">
+        <v>14</v>
+      </c>
+      <c r="IC50" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -36511,6 +36811,12 @@
       <c r="IA51" t="n">
         <v>34</v>
       </c>
+      <c r="IB51" t="n">
+        <v>36</v>
+      </c>
+      <c r="IC51" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -37220,6 +37526,12 @@
       <c r="IA52" t="n">
         <v>25</v>
       </c>
+      <c r="IB52" t="n">
+        <v>24</v>
+      </c>
+      <c r="IC52" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -37929,6 +38241,12 @@
       <c r="IA53" t="n">
         <v>34</v>
       </c>
+      <c r="IB53" t="n">
+        <v>33</v>
+      </c>
+      <c r="IC53" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -38638,6 +38956,12 @@
       <c r="IA54" t="n">
         <v>1</v>
       </c>
+      <c r="IB54" t="n">
+        <v>1</v>
+      </c>
+      <c r="IC54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -39347,6 +39671,12 @@
       <c r="IA55" t="n">
         <v>12</v>
       </c>
+      <c r="IB55" t="n">
+        <v>9</v>
+      </c>
+      <c r="IC55" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -40056,6 +40386,12 @@
       <c r="IA56" t="n">
         <v>80</v>
       </c>
+      <c r="IB56" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="IC56" t="n">
+        <v>85.7</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -40765,6 +41101,12 @@
       <c r="IA57" t="n">
         <v>120</v>
       </c>
+      <c r="IB57" t="n">
+        <v>142</v>
+      </c>
+      <c r="IC57" t="n">
+        <v>174</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -41474,6 +41816,12 @@
       <c r="IA58" t="n">
         <v>80</v>
       </c>
+      <c r="IB58" t="n">
+        <v>93</v>
+      </c>
+      <c r="IC58" t="n">
+        <v>104</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -42183,6 +42531,12 @@
       <c r="IA59" t="n">
         <v>200</v>
       </c>
+      <c r="IB59" t="n">
+        <v>235</v>
+      </c>
+      <c r="IC59" t="n">
+        <v>278</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -42892,6 +43246,12 @@
       <c r="IA60" t="n">
         <v>1.5</v>
       </c>
+      <c r="IB60" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="IC60" t="n">
+        <v>1.67</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -43601,6 +43961,12 @@
       <c r="IA61" t="n">
         <v>46</v>
       </c>
+      <c r="IB61" t="n">
+        <v>56</v>
+      </c>
+      <c r="IC61" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -44310,6 +44676,12 @@
       <c r="IA62" t="n">
         <v>50</v>
       </c>
+      <c r="IB62" t="n">
+        <v>53</v>
+      </c>
+      <c r="IC62" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -45019,6 +45391,12 @@
       <c r="IA63" t="n">
         <v>37</v>
       </c>
+      <c r="IB63" t="n">
+        <v>36</v>
+      </c>
+      <c r="IC63" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -45728,6 +46106,12 @@
       <c r="IA64" t="n">
         <v>10</v>
       </c>
+      <c r="IB64" t="n">
+        <v>13</v>
+      </c>
+      <c r="IC64" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -46437,6 +46821,12 @@
       <c r="IA65" t="n">
         <v>13</v>
       </c>
+      <c r="IB65" t="n">
+        <v>7</v>
+      </c>
+      <c r="IC65" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -47146,6 +47536,12 @@
       <c r="IA66" t="n">
         <v>5</v>
       </c>
+      <c r="IB66" t="n">
+        <v>6</v>
+      </c>
+      <c r="IC66" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -47855,6 +48251,12 @@
       <c r="IA67" t="n">
         <v>3</v>
       </c>
+      <c r="IB67" t="n">
+        <v>3</v>
+      </c>
+      <c r="IC67" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -48564,6 +48966,12 @@
       <c r="IA68" t="n">
         <v>2</v>
       </c>
+      <c r="IB68" t="n">
+        <v>6</v>
+      </c>
+      <c r="IC68" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -49273,6 +49681,12 @@
       <c r="IA69" t="n">
         <v>0</v>
       </c>
+      <c r="IB69" t="n">
+        <v>0</v>
+      </c>
+      <c r="IC69" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -49982,6 +50396,12 @@
       <c r="IA70" t="n">
         <v>7</v>
       </c>
+      <c r="IB70" t="n">
+        <v>12</v>
+      </c>
+      <c r="IC70" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -50691,6 +51111,12 @@
       <c r="IA71" t="n">
         <v>71.40000000000001</v>
       </c>
+      <c r="IB71" t="n">
+        <v>50</v>
+      </c>
+      <c r="IC71" t="n">
+        <v>57.1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -51400,6 +51826,12 @@
       <c r="IA72" t="n">
         <v>40</v>
       </c>
+      <c r="IB72" t="n">
+        <v>39.17</v>
+      </c>
+      <c r="IC72" t="n">
+        <v>23.17</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -52109,6 +52541,12 @@
       <c r="IA73" t="n">
         <v>28.57</v>
       </c>
+      <c r="IB73" t="n">
+        <v>19.58</v>
+      </c>
+      <c r="IC73" t="n">
+        <v>13.24</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -52818,6 +53256,12 @@
       <c r="IA74" t="n">
         <v>21</v>
       </c>
+      <c r="IB74" t="n">
+        <v>33</v>
+      </c>
+      <c r="IC74" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -53527,6 +53971,12 @@
       <c r="IA75" t="n">
         <v>48</v>
       </c>
+      <c r="IB75" t="n">
+        <v>41</v>
+      </c>
+      <c r="IC75" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -54236,6 +54686,12 @@
       <c r="IA76" t="n">
         <v>28</v>
       </c>
+      <c r="IB76" t="n">
+        <v>37</v>
+      </c>
+      <c r="IC76" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -54945,6 +55401,12 @@
       <c r="IA77" t="n">
         <v>30</v>
       </c>
+      <c r="IB77" t="n">
+        <v>32</v>
+      </c>
+      <c r="IC77" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -55654,6 +56116,12 @@
       <c r="IA78" t="n">
         <v>4.29</v>
       </c>
+      <c r="IB78" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="IC78" t="n">
+        <v>2.33</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -56363,6 +56831,12 @@
       <c r="IA79" t="n">
         <v>6</v>
       </c>
+      <c r="IB79" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="IC79" t="n">
+        <v>4.08</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -57072,6 +57546,12 @@
       <c r="IA80" t="n">
         <v>23.3</v>
       </c>
+      <c r="IB80" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="IC80" t="n">
+        <v>36.7</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -57781,6 +58261,12 @@
       <c r="IA81" t="n">
         <v>16.7</v>
       </c>
+      <c r="IB81" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="IC81" t="n">
+        <v>24.5</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -58490,6 +58976,12 @@
       <c r="IA82" t="n">
         <v>189.3</v>
       </c>
+      <c r="IB82" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="IC82" t="n">
+        <v>185.5</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -59199,6 +59691,12 @@
       <c r="IA83" t="n">
         <v>89</v>
       </c>
+      <c r="IB83" t="n">
+        <v>89.40000000000001</v>
+      </c>
+      <c r="IC83" t="n">
+        <v>86.2</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -59908,6 +60406,12 @@
       <c r="IA84" t="n">
         <v>26.8</v>
       </c>
+      <c r="IB84" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="IC84" t="n">
+        <v>27.8</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -60617,6 +61121,12 @@
       <c r="IA85" t="n">
         <v>112</v>
       </c>
+      <c r="IB85" t="n">
+        <v>114</v>
+      </c>
+      <c r="IC85" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -61326,6 +61836,12 @@
       <c r="IA86" t="n">
         <v>5</v>
       </c>
+      <c r="IB86" t="n">
+        <v>4</v>
+      </c>
+      <c r="IC86" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -62035,6 +62551,12 @@
       <c r="IA87" t="n">
         <v>5</v>
       </c>
+      <c r="IB87" t="n">
+        <v>7</v>
+      </c>
+      <c r="IC87" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -62744,6 +63266,12 @@
       <c r="IA88" t="n">
         <v>4</v>
       </c>
+      <c r="IB88" t="n">
+        <v>5</v>
+      </c>
+      <c r="IC88" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -63453,6 +63981,12 @@
       <c r="IA89" t="n">
         <v>8</v>
       </c>
+      <c r="IB89" t="n">
+        <v>6</v>
+      </c>
+      <c r="IC89" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -64162,6 +64696,12 @@
       <c r="IA90" t="n">
         <v>85</v>
       </c>
+      <c r="IB90" t="n">
+        <v>102</v>
+      </c>
+      <c r="IC90" t="n">
+        <v>124</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -64871,6 +65411,12 @@
       <c r="IA91" t="n">
         <v>109</v>
       </c>
+      <c r="IB91" t="n">
+        <v>112</v>
+      </c>
+      <c r="IC91" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -65580,6 +66126,12 @@
       <c r="IA92" t="n">
         <v>127</v>
       </c>
+      <c r="IB92" t="n">
+        <v>148</v>
+      </c>
+      <c r="IC92" t="n">
+        <v>173</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -66289,6 +66841,12 @@
       <c r="IA93" t="n">
         <v>63.5</v>
       </c>
+      <c r="IB93" t="n">
+        <v>63</v>
+      </c>
+      <c r="IC93" t="n">
+        <v>62.2</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -66998,6 +67556,12 @@
       <c r="IA94" t="n">
         <v>48</v>
       </c>
+      <c r="IB94" t="n">
+        <v>41</v>
+      </c>
+      <c r="IC94" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -67707,6 +68271,12 @@
       <c r="IA95" t="n">
         <v>8</v>
       </c>
+      <c r="IB95" t="n">
+        <v>13</v>
+      </c>
+      <c r="IC95" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -68416,6 +68986,12 @@
       <c r="IA96" t="n">
         <v>5</v>
       </c>
+      <c r="IB96" t="n">
+        <v>4</v>
+      </c>
+      <c r="IC96" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -69125,6 +69701,12 @@
       <c r="IA97" t="n">
         <v>21</v>
       </c>
+      <c r="IB97" t="n">
+        <v>33</v>
+      </c>
+      <c r="IC97" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -69834,6 +70416,12 @@
       <c r="IA98" t="n">
         <v>28</v>
       </c>
+      <c r="IB98" t="n">
+        <v>37</v>
+      </c>
+      <c r="IC98" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -70543,6 +71131,12 @@
       <c r="IA99" t="n">
         <v>35</v>
       </c>
+      <c r="IB99" t="n">
+        <v>32</v>
+      </c>
+      <c r="IC99" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -71252,6 +71846,12 @@
       <c r="IA100" t="n">
         <v>2</v>
       </c>
+      <c r="IB100" t="n">
+        <v>1</v>
+      </c>
+      <c r="IC100" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -71961,6 +72561,12 @@
       <c r="IA101" t="n">
         <v>3</v>
       </c>
+      <c r="IB101" t="n">
+        <v>3</v>
+      </c>
+      <c r="IC101" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -72670,8 +73276,14 @@
       <c r="IA102" t="n">
         <v>60</v>
       </c>
+      <c r="IB102" t="n">
+        <v>50</v>
+      </c>
+      <c r="IC102" t="n">
+        <v>83.3</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>